<commit_message>
Updated code with GUI
</commit_message>
<xml_diff>
--- a/aggregated_output.xlsx
+++ b/aggregated_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,60 +551,75 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
+          <t>Jahr</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
           <t>Zur Promotion berechtigende</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Art des Abschlusses</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>In welchem Studiengang wurden Sie geprüft</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Mit welcher Gesamtnote wurde die Prüfung beurteilt?</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Wo erwarben Sie den Hochschulabschluss?</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Bitte geben Sie das Kfz-Kennzeichen des Erwerbsortes an?</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Wann wurde das Prüfungsergebnis offiziell festgestellt?</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Fachgebiet</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Art der Promotion</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Art der Dissertation</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Teilnahme an einem strukturierten Promotionsprogramm</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Thema der Dissertation</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Betreuer/in der Dissertation</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Datum</t>
         </is>
@@ -728,60 +743,76 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>Master of Science</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>Elektro- und Informationstechnik</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>1,1</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>KA</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>25042019</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Certifiable Multiple Object Tracking for Autonomous Systems+(Zertifizierbares Multiple Object Tracking für Autonome Systeme)</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>Prof. Dr.-Ing. Benjamin Noack</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>19.04.2022</t>
         </is>
@@ -901,60 +932,75 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>Diplom</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AB3" t="inlineStr">
         <is>
           <t>1,4</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>MD</t>
         </is>
       </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>151097</t>
         </is>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AF3" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>Microcredentials für den Kompetenzerwerb im Bereich Datenbewusstsein und informaitonelle Selbstbestimmung</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>Prof. Andreas Nürnberger</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>15.06.2023</t>
         </is>
@@ -1074,68 +1120,95 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>Master</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AB4" t="inlineStr">
         <is>
           <t>1,3</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="AC4" t="inlineStr">
+      <c r="AD4" t="inlineStr">
         <is>
           <t>MD</t>
         </is>
       </c>
-      <c r="AD4" t="inlineStr">
+      <c r="AE4" t="inlineStr">
         <is>
           <t>16092021</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AF4" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
         <is>
           <t>kumulativ</t>
         </is>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AI4" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>Acceleration of numerical simulations including sea-ice and fluid dynamics with graphics processing units and machine learning.</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
         <is>
           <t>Jun. Prof. Christian Lessig</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Heise</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Julia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01031995</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>W</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1168,47 +1241,142 @@
           <t>julia.heise@ovgu.de</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t xml:space="preserve">   </t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
+          <t>Gymnasium (aHR)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>29062013</t>
+        </is>
+      </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Nordrhein-Westfalen</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Otto-von-Guericke-Universität Magdeburg</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Informatik</t>
+        </is>
+      </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>25022022</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Multi-Objective Evolutionary Algorithms</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>Monografie</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>Nein</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>Development of Robust Multi-Objective Optimization and Decision-Making Algorithms</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>Prof. Dr.-Ing. habil. Sanaz Mostaghim</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>04.10.2022</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1324,60 +1492,75 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
           <t>Ja</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
         <is>
           <t>Master of Science</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
+      <c r="AA6" t="inlineStr">
         <is>
           <t>Digital Engineering</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AB6" t="inlineStr">
         <is>
           <t>1,1</t>
         </is>
       </c>
-      <c r="AB6" t="inlineStr">
+      <c r="AC6" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="AC6" t="inlineStr">
+      <c r="AD6" t="inlineStr">
         <is>
           <t>MD</t>
         </is>
       </c>
-      <c r="AD6" t="inlineStr">
+      <c r="AE6" t="inlineStr">
         <is>
           <t>01.04.2021</t>
         </is>
       </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AF6" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AF6" t="inlineStr">
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AI6" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AH6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>Understanding Evolutionary Patterns in the Architectural Degradation of Software‐System Quality</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>Dr.-Ing. habil. Sandro Schulze</t>
         </is>
       </c>
-      <c r="AI6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated some tables according to the intended outputs
</commit_message>
<xml_diff>
--- a/aggregated_output.xlsx
+++ b/aggregated_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:AM6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,52 +486,52 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Staatsangehörigkeit(1)</t>
+          <t>Staatsangehörigkeit</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Staatsangehörigkeit(2)</t>
+          <t>Weitere Staatsangehörigkeit</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Einschreibung</t>
+          <t>Einschreibung als Promotionsstudierenden</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Besteht eine Behinderung</t>
+          <t>Beschäftigungsverhältnis mit OVGU / Klinikum</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Welche art der Behinderung</t>
+          <t>Art der HZB</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Wann erwarben Sie die Behinderung</t>
+          <t>Datum HZB-Erwerb</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Wo erwarben Sie die Behinderung</t>
+          <t>Staat HZB-Erwerb</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Wo erwarben Sie die Behinderung?</t>
+          <t>Landkreis HZB-Erwerb</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Bitte geben Sie an, ob Sie eine der folgenden Leistungen beziehen:</t>
+          <t>Staat der Ersteinschreibung</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Wo erfolgte die Hochschulzugangsberechtigung?</t>
+          <t>Wo erfolgte die Hochschulzugangsberechtigung</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
@@ -541,87 +541,92 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>Hochschule der Ersteinschreibung (falls Inland)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Monat</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Jahr</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Zur Promotion berechtigende</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Art des Abschlusses</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>In welchem Studiengang wurden Sie geprüft</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Mit welcher Gesamtnote wurde die Prüfung beurteilt?</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Wo erwarben Sie den Hochschulabschluss?</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Bitte geben Sie das Kfz-Kennzeichen des Erwerbsortes an?</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
           <t>Bezeichnung der Hochschuleinrichtung</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Monat</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Jahr</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Zur Promotion berechtigende</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Art des Abschlusses</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>In welchem Studiengang wurden Sie geprüft</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Mit welcher Gesamtnote wurde die Prüfung beurteilt?</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Wo erwarben Sie den Hochschulabschluss?</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Bitte geben Sie das Kfz-Kennzeichen des Erwerbsortes an?</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Wann wurde das Prüfungsergebnis offiziell festgestellt?</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Fachgebiet</t>
-        </is>
-      </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
+          <t>Fachgebiet der Promotion</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
           <t>Art der Promotion</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Art der Dissertation</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Teilnahme an einem strukturierten Promotionsprogramm</t>
-        </is>
-      </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Thema der Dissertation</t>
+          <t>Teilnahme an strukturiertem Promotionsprogramm</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Betreuer/in der Dissertation</t>
+          <t>Thema</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Datum</t>
+          <t>Betreuer</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Datum der Zulassung</t>
         </is>
       </c>
     </row>
@@ -778,41 +783,46 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
+          <t>Karlsruher Institut für Technologie</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
           <t>25042019</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>Certifiable Multiple Object Tracking for Autonomous Systems (Zertifizierbares Multiple Object Tracking für Autonome Systeme)</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>Prof. Dr.-Ing. Benjamin Noack</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>19.04.2022</t>
         </is>
@@ -922,85 +932,90 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
+          <t>Hochschule für Ökonomie Berlin</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Diplom</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Informatik</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
           <t>Otto-von-Guericke-Universität</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>09</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Diplom</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>151097</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>1,4</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>MD</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>151097</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>Informatik</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AJ3" t="inlineStr">
+      <c r="AK3" t="inlineStr">
         <is>
           <t>Microcredentials für den Kompetenzerwerb im Bereich Datenbewusstsein und informaitonelle Selbstbestimmung</t>
         </is>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>Prof. Andreas Nürnberger</t>
         </is>
       </c>
-      <c r="AL3" t="inlineStr">
+      <c r="AM3" t="inlineStr">
         <is>
           <t>15.06.2023</t>
         </is>
@@ -1155,40 +1170,45 @@
       </c>
       <c r="AE4" t="inlineStr">
         <is>
+          <t>Otto-von-Guericke-Universität</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
           <t>16092021</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
+      <c r="AG4" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AI4" t="inlineStr">
         <is>
           <t>kumulativ</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AJ4" t="inlineStr">
+      <c r="AK4" t="inlineStr">
         <is>
           <t>Acceleration of numerical simulations including sea-ice and fluid dynamics with graphics processing units and machine learning.</t>
         </is>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AL4" t="inlineStr">
         <is>
           <t>Jun. Prof. Christian Lessig</t>
         </is>
       </c>
-      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1339,40 +1359,45 @@
       </c>
       <c r="AE5" t="inlineStr">
         <is>
+          <t>Otto-von-Guericke-Universität Magdeburg</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
           <t>25022022</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr">
+      <c r="AG5" t="inlineStr">
         <is>
           <t>Multi-Objective Evolutionary Algorithms</t>
         </is>
       </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AH5" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AI5" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AI5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AK5" t="inlineStr">
         <is>
           <t>Development of Robust Multi-Objective Optimization and Decision-Making Algorithms</t>
         </is>
       </c>
-      <c r="AK5" t="inlineStr">
+      <c r="AL5" t="inlineStr">
         <is>
           <t>Prof. Dr.-Ing. habil. Sanaz Mostaghim</t>
         </is>
       </c>
-      <c r="AL5" t="inlineStr">
+      <c r="AM5" t="inlineStr">
         <is>
           <t>04.10.2022</t>
         </is>
@@ -1482,85 +1507,90 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
+          <t>Hochschule für Angewandte Wissenschaften Hof</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Master of Science</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>Digital Engineering</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
           <t>Otto-von-Guericke-Universität Magdeburg</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Ja</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Master of Science</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>Digital Engineering</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>1,1</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>MD</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AF6" t="inlineStr">
         <is>
           <t>01.04.2021</t>
         </is>
       </c>
-      <c r="AF6" t="inlineStr">
+      <c r="AG6" t="inlineStr">
         <is>
           <t>Informatik</t>
         </is>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AH6" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
-      <c r="AH6" t="inlineStr">
+      <c r="AI6" t="inlineStr">
         <is>
           <t>Monografie</t>
         </is>
       </c>
-      <c r="AI6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>Nein</t>
         </is>
       </c>
-      <c r="AJ6" t="inlineStr">
+      <c r="AK6" t="inlineStr">
         <is>
           <t>Understanding Evolutionary Patterns in the Architectural Degradation of Software‐System Quality</t>
         </is>
       </c>
-      <c r="AK6" t="inlineStr">
+      <c r="AL6" t="inlineStr">
         <is>
           <t>Dr.-Ing. habil. Sandro Schulze</t>
         </is>
       </c>
-      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>